<commit_message>
added spreadsheet->yaml to workflow
</commit_message>
<xml_diff>
--- a/tests/sample_prompts.xlsx
+++ b/tests/sample_prompts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisyd-my.sharepoint.com/personal/xinwei_luo_sydney_edu_au/Documents/work/PIPE-3692-Costs of Litigation - Inheritance and Class Action/langchainlaw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisyd-my.sharepoint.com/personal/xinwei_luo_sydney_edu_au/Documents/work/PIPE-3692-Costs of Litigation - Inheritance and Class Action/langchainlaw/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{8E48C5E2-382D-5045-8C4C-8FDEDCDC88D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80B43C5-C193-924D-BD3E-77CDDBC5462C}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{8E48C5E2-382D-5045-8C4C-8FDEDCDC88D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1227929B-6E30-4443-B48B-A9A4EDB89E43}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_prompts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="122">
   <si>
     <t>Prompt_name</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>fields</t>
-  </si>
-  <si>
-    <t>question_number</t>
   </si>
   <si>
     <t>question_description</t>
@@ -1269,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059D518-D0B8-2E48-ACAE-8A1C600718FA}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="116" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,10 +1283,9 @@
     <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="173.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="162.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,715 +1293,604 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
       </c>
       <c r="I2" s="1">
         <v>40334</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
       </c>
       <c r="I4" s="1">
         <v>40241</v>
       </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
       </c>
       <c r="I6" s="1">
         <v>39570</v>
       </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="I7" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
         <v>114</v>
       </c>
-      <c r="L7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
         <v>108</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="L12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="238" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
         <v>109</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" t="s">
-        <v>115</v>
-      </c>
-      <c r="L14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" t="s">
-        <v>109</v>
-      </c>
-      <c r="L15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
         <v>45</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
         <v>110</v>
       </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" t="s">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>47</v>
       </c>
-      <c r="I17" t="s">
-        <v>111</v>
-      </c>
-      <c r="L17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>48</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
         <v>49</v>
       </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>50</v>
-      </c>
-      <c r="H19" t="s">
-        <v>51</v>
       </c>
       <c r="I19" s="1">
         <v>39971</v>
       </c>
-      <c r="L19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="s">
         <v>116</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
         <v>56</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" t="s">
         <v>117</v>
       </c>
-      <c r="L21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" t="s">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" t="s">
         <v>58</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H23" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I24" t="s">
         <v>118</v>
       </c>
-      <c r="L22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" t="s">
-        <v>109</v>
-      </c>
-      <c r="L23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" t="s">
+    </row>
+    <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c r="I24" t="s">
-        <v>119</v>
-      </c>
-      <c r="L24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="238" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" t="s">
         <v>65</v>
       </c>
-      <c r="I25" t="s">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="s">
         <v>66</v>
       </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>67</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" t="s">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" t="s">
         <v>69</v>
       </c>
-      <c r="L26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>70</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>71</v>
       </c>
-      <c r="I27" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" t="s">
         <v>72</v>
       </c>
-      <c r="L27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>73</v>
-      </c>
-      <c r="H28" t="s">
-        <v>74</v>
       </c>
       <c r="I28" s="3">
         <v>20000</v>
       </c>
-      <c r="L28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
         <v>75</v>
-      </c>
-      <c r="H29" t="s">
-        <v>76</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
       </c>
-      <c r="L29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
         <v>77</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s">
         <v>78</v>
       </c>
-      <c r="I30" t="s">
-        <v>113</v>
-      </c>
-      <c r="L30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>79</v>
-      </c>
-      <c r="H31" t="s">
-        <v>80</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
-      <c r="L31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
-      <c r="L32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" t="s">
         <v>82</v>
-      </c>
-      <c r="H33" t="s">
-        <v>83</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
-      <c r="L33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" t="s">
         <v>84</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" t="s">
         <v>85</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H35" t="s">
+        <v>86</v>
+      </c>
+      <c r="I35" t="s">
         <v>120</v>
       </c>
-      <c r="L34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G35" t="s">
-        <v>86</v>
-      </c>
-      <c r="H35" t="s">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" t="s">
         <v>87</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H36" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" t="s">
         <v>121</v>
       </c>
-      <c r="L35">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" t="s">
-        <v>88</v>
-      </c>
-      <c r="H36" t="s">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G37" t="s">
         <v>89</v>
       </c>
-      <c r="I36" t="s">
-        <v>122</v>
-      </c>
-      <c r="L36">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>90</v>
-      </c>
-      <c r="H37" t="s">
-        <v>91</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
-      </c>
-      <c r="L37">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2029,12 +1914,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2054,12 +1939,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still refactoring the prompt classes
</commit_message>
<xml_diff>
--- a/tests/sample_prompts.xlsx
+++ b/tests/sample_prompts.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisyd-my.sharepoint.com/personal/xinwei_luo_sydney_edu_au/Documents/work/PIPE-3692-Costs of Litigation - Inheritance and Class Action/langchainlaw/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/langchainlaw/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{8E48C5E2-382D-5045-8C4C-8FDEDCDC88D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1227929B-6E30-4443-B48B-A9A4EDB89E43}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C20BF1-E135-1A4F-9F0E-00E07C564531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
   </bookViews>
   <sheets>
-    <sheet name="sample_prompts" sheetId="1" r:id="rId1"/>
+    <sheet name="prompts" sheetId="1" r:id="rId1"/>
     <sheet name="system" sheetId="2" r:id="rId2"/>
     <sheet name="intro" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8059D518-D0B8-2E48-ACAE-8A1C600718FA}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1704,7 +1704,7 @@
         <v>63</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Cleaned up a typo in the test spreadsheet
</commit_message>
<xml_diff>
--- a/tests/sample_prompts.xlsx
+++ b/tests/sample_prompts.xlsx
@@ -8,16 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/langchainlaw/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C20BF1-E135-1A4F-9F0E-00E07C564531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D667FA7-51F4-BA40-9A2B-DFE5CB34787E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
+    <workbookView xWindow="0" yWindow="8300" windowWidth="54220" windowHeight="20500" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts" sheetId="1" r:id="rId1"/>
     <sheet name="system" sheetId="2" r:id="rId2"/>
     <sheet name="intro" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,9 +62,6 @@
   </si>
   <si>
     <t>interlocutory</t>
-  </si>
-  <si>
-    <t>Does this judgment concern an interlocutory applicatidoes this judgment concern an interlocutory application? Answer "yes", "no" or "unclear" on?</t>
   </si>
   <si>
     <t>yes</t>
@@ -398,6 +408,9 @@
   </si>
   <si>
     <t xml:space="preserve">the party threatened the plaintiff </t>
+  </si>
+  <si>
+    <t>Does this judgment concern an interlocutory applicatidoes this judgment concern an interlocutory application? Answer "yes", "no" or "unclear"</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1282,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,16 +1306,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1311,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1322,10 +1335,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1345,10 +1358,10 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
         <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1356,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
       </c>
       <c r="I4" s="1">
         <v>40241</v>
@@ -1367,36 +1380,36 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
         <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
       </c>
       <c r="I6" s="1">
         <v>39570</v>
@@ -1404,211 +1417,211 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="H11" t="s">
-        <v>32</v>
-      </c>
       <c r="I11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
         <v>39</v>
       </c>
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
         <v>41</v>
       </c>
-      <c r="H15" t="s">
-        <v>42</v>
-      </c>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" t="s">
         <v>43</v>
       </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
       <c r="I16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
         <v>45</v>
       </c>
-      <c r="H17" t="s">
-        <v>46</v>
-      </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
         <v>47</v>
       </c>
-      <c r="H18" t="s">
-        <v>48</v>
-      </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
         <v>49</v>
-      </c>
-      <c r="H19" t="s">
-        <v>50</v>
       </c>
       <c r="I19" s="1">
         <v>39971</v>
@@ -1616,152 +1629,152 @@
     </row>
     <row r="20" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
         <v>52</v>
       </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
       <c r="I20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
         <v>54</v>
       </c>
-      <c r="H21" t="s">
-        <v>55</v>
-      </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
         <v>56</v>
       </c>
-      <c r="H22" t="s">
-        <v>57</v>
-      </c>
       <c r="I22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" t="s">
         <v>58</v>
       </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
       <c r="I23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
         <v>60</v>
       </c>
-      <c r="H24" t="s">
-        <v>61</v>
-      </c>
       <c r="I24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" t="s">
         <v>64</v>
-      </c>
-      <c r="I25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" t="s">
         <v>66</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>67</v>
-      </c>
-      <c r="I26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" t="s">
         <v>69</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>70</v>
-      </c>
-      <c r="I27" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" t="s">
         <v>72</v>
-      </c>
-      <c r="H28" t="s">
-        <v>73</v>
       </c>
       <c r="I28" s="3">
         <v>20000</v>
@@ -1769,13 +1782,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
         <v>74</v>
-      </c>
-      <c r="H29" t="s">
-        <v>75</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1783,27 +1796,27 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" t="s">
         <v>76</v>
       </c>
-      <c r="H30" t="s">
-        <v>77</v>
-      </c>
       <c r="I30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" t="s">
         <v>78</v>
-      </c>
-      <c r="H31" t="s">
-        <v>79</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -1811,13 +1824,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -1825,13 +1838,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" t="s">
         <v>81</v>
-      </c>
-      <c r="H33" t="s">
-        <v>82</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
@@ -1839,55 +1852,55 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" t="s">
         <v>83</v>
       </c>
-      <c r="H34" t="s">
-        <v>84</v>
-      </c>
       <c r="I34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" t="s">
         <v>85</v>
       </c>
-      <c r="H35" t="s">
-        <v>86</v>
-      </c>
       <c r="I35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" t="s">
+        <v>86</v>
+      </c>
+      <c r="H36" t="s">
         <v>87</v>
       </c>
-      <c r="H36" t="s">
-        <v>88</v>
-      </c>
       <c r="I36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" t="s">
         <v>89</v>
-      </c>
-      <c r="H37" t="s">
-        <v>90</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -1914,12 +1927,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1939,12 +1952,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated documentation with --no-cache and --test flags for the command-line tool
</commit_message>
<xml_diff>
--- a/tests/sample_prompts.xlsx
+++ b/tests/sample_prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/langchainlaw/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D667FA7-51F4-BA40-9A2B-DFE5CB34787E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCBA1DB-696F-1D4B-AC63-61AE5505E555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8300" windowWidth="54220" windowHeight="20500" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
+    <workbookView xWindow="2400" yWindow="800" windowWidth="33600" windowHeight="20500" xr2:uid="{631EE46B-1F17-3D48-9EF2-EF10E6A7DFED}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>